<commit_message>
functional changes in the code
</commit_message>
<xml_diff>
--- a/testData.xlsx
+++ b/testData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -31,6 +31,18 @@
     <t>Pnr</t>
   </si>
   <si>
+    <t>Firstname</t>
+  </si>
+  <si>
+    <t>Lastname</t>
+  </si>
+  <si>
+    <t>Departure</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
     <t>abc</t>
   </si>
   <si>
@@ -43,7 +55,19 @@
     <t>amadeus12</t>
   </si>
   <si>
-    <t>OT9MKP</t>
+    <t>OYJWIU</t>
+  </si>
+  <si>
+    <t>AIRCANADATEST</t>
+  </si>
+  <si>
+    <t>AMERICAN</t>
+  </si>
+  <si>
+    <t>YYZ</t>
+  </si>
+  <si>
+    <t>abc@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -51,10 +75,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -81,9 +105,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -91,9 +129,16 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -105,25 +150,63 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -136,66 +219,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -218,19 +242,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -242,163 +380,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -412,26 +436,28 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -460,15 +486,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -486,26 +503,33 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -514,7 +538,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -532,130 +556,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -991,17 +1015,19 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="23.7142857142857" customWidth="1"/>
-    <col min="10" max="10" width="11.7142857142857"/>
+    <col min="3" max="3" width="13.1428571428571" customWidth="1"/>
+    <col min="4" max="4" width="10.7142857142857" customWidth="1"/>
+    <col min="10" max="10" width="20.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1016,32 +1042,53 @@
       </c>
       <c r="E1" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2"/>
-      <c r="G2"/>
-      <c r="H2"/>
-      <c r="I2" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="https://pssuat.aircanada.com/ca/en/aco/home.html#" tooltip="https://pssuat.aircanada.com/ca/en/aco/home.html#"/>
+    <hyperlink ref="I2" r:id="rId2" display="abc@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>